<commit_message>
Fix a bug what cannot get the nic combo version
</commit_message>
<xml_diff>
--- a/SystemAutomation.xlsx
+++ b/SystemAutomation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\MyLab\Dsas_Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\UiPath\Dsas_Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AC1ACB-D329-455C-8E37-2EEE857C46D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C1DBC7-3443-4F2B-90A9-6F9BE1773954}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="885" yWindow="-120" windowWidth="19725" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2565" yWindow="1560" windowWidth="17295" windowHeight="8325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HPE_Server" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="291">
   <si>
     <t>P06687-B21</t>
   </si>
@@ -947,6 +947,10 @@
   </si>
   <si>
     <t>https://support.hpe.com/hpsc/swd/public/detail?swItemId=MTX_379daccdc547448493fd2c5b17&amp;swEnvOid=4176</t>
+    <phoneticPr fontId="19"/>
+  </si>
+  <si>
+    <t>https://support.hpe.com/hpsc/swd/public/detail?swItemId=MTX_d44f26458a5c435982ed57b5dc&amp;swEnvOid=4176</t>
     <phoneticPr fontId="19"/>
   </si>
 </sst>
@@ -1331,7 +1335,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1444,6 +1448,9 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
@@ -1453,7 +1460,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -5070,8 +5077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -5126,7 +5133,7 @@
       <c r="C3" s="21" t="s">
         <v>286</v>
       </c>
-      <c r="D3" s="59" t="s">
+      <c r="D3" s="56" t="s">
         <v>289</v>
       </c>
       <c r="E3" s="52" t="s">
@@ -5218,7 +5225,9 @@
       <c r="C8" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="49"/>
+      <c r="D8" s="60" t="s">
+        <v>290</v>
+      </c>
       <c r="E8" s="52" t="s">
         <v>283</v>
       </c>
@@ -5231,7 +5240,7 @@
       <c r="C9" s="8" t="s">
         <v>286</v>
       </c>
-      <c r="D9" s="59" t="s">
+      <c r="D9" s="56" t="s">
         <v>289</v>
       </c>
       <c r="E9" s="53" t="s">
@@ -5265,7 +5274,7 @@
       <c r="C11" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="D11" s="59" t="s">
+      <c r="D11" s="56" t="s">
         <v>289</v>
       </c>
       <c r="E11" s="52" t="s">
@@ -6722,9 +6731,10 @@
     <hyperlink ref="D3" r:id="rId6" xr:uid="{7762A748-BFB8-4C5E-95AF-42B3B014EC57}"/>
     <hyperlink ref="D9" r:id="rId7" xr:uid="{4B79DC39-E24D-48B6-A7DC-461E8CB5E390}"/>
     <hyperlink ref="D11" r:id="rId8" xr:uid="{840EBDFF-FD91-4136-A19A-863BCDE17DD0}"/>
+    <hyperlink ref="D8" r:id="rId9" xr:uid="{745829DE-603C-44D1-A7C4-3EB3DE205FC0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId9"/>
+  <pageSetup orientation="landscape" r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -10190,10 +10200,10 @@
       <c r="I10" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="J10" s="56" t="s">
+      <c r="J10" s="57" t="s">
         <v>157</v>
       </c>
-      <c r="K10" s="57"/>
+      <c r="K10" s="58"/>
       <c r="L10" s="5" t="s">
         <v>161</v>
       </c>
@@ -14337,10 +14347,10 @@
     </row>
     <row r="5" spans="2:7" ht="18.75" customHeight="1"/>
     <row r="6" spans="2:7" ht="18.75" customHeight="1">
-      <c r="D6" s="58" t="s">
+      <c r="D6" s="59" t="s">
         <v>276</v>
       </c>
-      <c r="E6" s="57"/>
+      <c r="E6" s="58"/>
       <c r="F6" s="6" t="s">
         <v>277</v>
       </c>

</xml_diff>